<commit_message>
results policis on N7
</commit_message>
<xml_diff>
--- a/table_results_policies.xlsx
+++ b/table_results_policies.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="93">
   <si>
     <t>name</t>
   </si>
@@ -167,6 +167,132 @@
   </si>
   <si>
     <t>I2_N5_T100_C200_0_P6</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0_P1</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0_P2</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0_P3</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0_P4</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0_P5</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C140_0_P6</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0_P1</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0_P2</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0_P3</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0_P4</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0_P5</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C210_0_P6</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0_P1</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0_P2</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0_P3</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0_P4</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0_P5</t>
+  </si>
+  <si>
+    <t>I2_N7_T30_C280_0_P6</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0_P1</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0_P2</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0_P3</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0_P4</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0_P5</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C140_0_P6</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0_P1</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0_P2</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0_P3</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0_P4</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0_P5</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C210_0_P6</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0_P1</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0_P2</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0_P3</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0_P4</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0_P5</t>
+  </si>
+  <si>
+    <t>I2_N7_T100_C280_0_P6</t>
   </si>
 </sst>
 </file>
@@ -524,7 +650,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:J85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1903,6 +2029,1350 @@
         <v>0</v>
       </c>
     </row>
+    <row r="44" spans="1:10">
+      <c r="A44" s="1">
+        <v>42</v>
+      </c>
+      <c r="B44" t="s">
+        <v>51</v>
+      </c>
+      <c r="C44">
+        <v>309.431978056256</v>
+      </c>
+      <c r="D44">
+        <v>2.366000175476074</v>
+      </c>
+      <c r="E44">
+        <v>0.9693721510508347</v>
+      </c>
+      <c r="F44">
+        <v>33.86197805599477</v>
+      </c>
+      <c r="G44">
+        <v>0</v>
+      </c>
+      <c r="H44">
+        <v>0</v>
+      </c>
+      <c r="I44">
+        <v>225.2600000002612</v>
+      </c>
+      <c r="J44">
+        <v>50.31</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10">
+      <c r="A45" s="1">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>52</v>
+      </c>
+      <c r="C45">
+        <v>1019.699639895617</v>
+      </c>
+      <c r="D45">
+        <v>0.01200008392333984</v>
+      </c>
+      <c r="E45">
+        <v>0</v>
+      </c>
+      <c r="F45">
+        <v>26.35557902654179</v>
+      </c>
+      <c r="G45">
+        <v>7.118526273374133</v>
+      </c>
+      <c r="H45">
+        <v>5.792587142453418</v>
+      </c>
+      <c r="I45">
+        <v>941.5899999999959</v>
+      </c>
+      <c r="J45">
+        <v>53.08</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10">
+      <c r="A46" s="1">
+        <v>44</v>
+      </c>
+      <c r="B46" t="s">
+        <v>53</v>
+      </c>
+      <c r="C46">
+        <v>396.5896102867711</v>
+      </c>
+      <c r="D46">
+        <v>0.01600003242492676</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+      <c r="F46">
+        <v>27.5296102867676</v>
+      </c>
+      <c r="G46">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="H46">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="I46">
+        <v>275.5500000000035</v>
+      </c>
+      <c r="J46">
+        <v>93.50999999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10">
+      <c r="A47" s="1">
+        <v>45</v>
+      </c>
+      <c r="B47" t="s">
+        <v>54</v>
+      </c>
+      <c r="C47">
+        <v>396.5896102867718</v>
+      </c>
+      <c r="D47">
+        <v>0.02200007438659668</v>
+      </c>
+      <c r="E47">
+        <v>0</v>
+      </c>
+      <c r="F47">
+        <v>27.5296102867676</v>
+      </c>
+      <c r="G47">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="H47">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="I47">
+        <v>275.5500000000042</v>
+      </c>
+      <c r="J47">
+        <v>93.50999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10">
+      <c r="A48" s="1">
+        <v>46</v>
+      </c>
+      <c r="B48" t="s">
+        <v>55</v>
+      </c>
+      <c r="C48">
+        <v>357.599157859413</v>
+      </c>
+      <c r="D48">
+        <v>0.01700019836425781</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>33.10915785941906</v>
+      </c>
+      <c r="G48">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="H48">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="I48">
+        <v>264.119999999994</v>
+      </c>
+      <c r="J48">
+        <v>60.37</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10">
+      <c r="A49" s="1">
+        <v>47</v>
+      </c>
+      <c r="B49" t="s">
+        <v>56</v>
+      </c>
+      <c r="C49">
+        <v>1021.419132648</v>
+      </c>
+      <c r="D49">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>26.74913264799307</v>
+      </c>
+      <c r="G49">
+        <v>4.450188684067006</v>
+      </c>
+      <c r="H49">
+        <v>4.450188684067006</v>
+      </c>
+      <c r="I49">
+        <v>393.770000000007</v>
+      </c>
+      <c r="J49">
+        <v>600.9000000000001</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10">
+      <c r="A50" s="1">
+        <v>48</v>
+      </c>
+      <c r="B50" t="s">
+        <v>57</v>
+      </c>
+      <c r="C50">
+        <v>696.9392770648811</v>
+      </c>
+      <c r="D50">
+        <v>0.00800013542175293</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>36.70927706488092</v>
+      </c>
+      <c r="G50">
+        <v>4.738617941974221</v>
+      </c>
+      <c r="H50">
+        <v>4.738617941974221</v>
+      </c>
+      <c r="I50">
+        <v>428.3500000000003</v>
+      </c>
+      <c r="J50">
+        <v>231.88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10">
+      <c r="A51" s="1">
+        <v>49</v>
+      </c>
+      <c r="B51" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51">
+        <v>26.53458309510687</v>
+      </c>
+      <c r="D51">
+        <v>0.9140000343322754</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+      <c r="F51">
+        <v>26.53458309510687</v>
+      </c>
+      <c r="G51">
+        <v>0</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>0</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10">
+      <c r="A52" s="1">
+        <v>50</v>
+      </c>
+      <c r="B52" t="s">
+        <v>59</v>
+      </c>
+      <c r="C52">
+        <v>1091.229339571343</v>
+      </c>
+      <c r="D52">
+        <v>0.009000062942504883</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+      <c r="F52">
+        <v>23.91796089943222</v>
+      </c>
+      <c r="G52">
+        <v>4.77723927008741</v>
+      </c>
+      <c r="H52">
+        <v>4.738617941974221</v>
+      </c>
+      <c r="I52">
+        <v>620.2700000000234</v>
+      </c>
+      <c r="J52">
+        <v>447.08</v>
+      </c>
+    </row>
+    <row r="53" spans="1:10">
+      <c r="A53" s="1">
+        <v>51</v>
+      </c>
+      <c r="B53" t="s">
+        <v>60</v>
+      </c>
+      <c r="C53">
+        <v>497.0523554984831</v>
+      </c>
+      <c r="D53">
+        <v>0.01600003242492676</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G53">
+        <v>6.065177049722176</v>
+      </c>
+      <c r="H53">
+        <v>2.836886568752553</v>
+      </c>
+      <c r="I53">
+        <v>366.5900000000053</v>
+      </c>
+      <c r="J53">
+        <v>108.7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:10">
+      <c r="A54" s="1">
+        <v>52</v>
+      </c>
+      <c r="B54" t="s">
+        <v>61</v>
+      </c>
+      <c r="C54">
+        <v>500.280645979443</v>
+      </c>
+      <c r="D54">
+        <v>0.0130000114440918</v>
+      </c>
+      <c r="E54">
+        <v>0</v>
+      </c>
+      <c r="F54">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G54">
+        <v>2.378003364169193</v>
+      </c>
+      <c r="H54">
+        <v>2.378003364169193</v>
+      </c>
+      <c r="I54">
+        <v>422.4199999999955</v>
+      </c>
+      <c r="J54">
+        <v>52.87</v>
+      </c>
+    </row>
+    <row r="55" spans="1:10">
+      <c r="A55" s="1">
+        <v>53</v>
+      </c>
+      <c r="B55" t="s">
+        <v>62</v>
+      </c>
+      <c r="C55">
+        <v>135.0555790265418</v>
+      </c>
+      <c r="D55">
+        <v>0.006000041961669922</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+      <c r="F55">
+        <v>26.35557902654179</v>
+      </c>
+      <c r="G55">
+        <v>0</v>
+      </c>
+      <c r="H55">
+        <v>0</v>
+      </c>
+      <c r="I55">
+        <v>0</v>
+      </c>
+      <c r="J55">
+        <v>108.7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:10">
+      <c r="A56" s="1">
+        <v>54</v>
+      </c>
+      <c r="B56" t="s">
+        <v>63</v>
+      </c>
+      <c r="C56">
+        <v>1091.43471156119</v>
+      </c>
+      <c r="D56">
+        <v>0.006999969482421875</v>
+      </c>
+      <c r="E56">
+        <v>0</v>
+      </c>
+      <c r="F56">
+        <v>24.3115145208835</v>
+      </c>
+      <c r="G56">
+        <v>3.366602695185008</v>
+      </c>
+      <c r="H56">
+        <v>3.139799735480239</v>
+      </c>
+      <c r="I56">
+        <v>969.9100000000115</v>
+      </c>
+      <c r="J56">
+        <v>97.44</v>
+      </c>
+    </row>
+    <row r="57" spans="1:10">
+      <c r="A57" s="1">
+        <v>55</v>
+      </c>
+      <c r="B57" t="s">
+        <v>64</v>
+      </c>
+      <c r="C57">
+        <v>147.3892770648809</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+      <c r="F57">
+        <v>36.70927706488092</v>
+      </c>
+      <c r="G57">
+        <v>0</v>
+      </c>
+      <c r="H57">
+        <v>0</v>
+      </c>
+      <c r="I57">
+        <v>0</v>
+      </c>
+      <c r="J57">
+        <v>110.68</v>
+      </c>
+    </row>
+    <row r="58" spans="1:10">
+      <c r="A58" s="1">
+        <v>56</v>
+      </c>
+      <c r="B58" t="s">
+        <v>65</v>
+      </c>
+      <c r="C58">
+        <v>26.29875013250022</v>
+      </c>
+      <c r="D58">
+        <v>1.130999803543091</v>
+      </c>
+      <c r="E58">
+        <v>0</v>
+      </c>
+      <c r="F58">
+        <v>26.29875013250022</v>
+      </c>
+      <c r="G58">
+        <v>0</v>
+      </c>
+      <c r="H58">
+        <v>0</v>
+      </c>
+      <c r="I58">
+        <v>0</v>
+      </c>
+      <c r="J58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:10">
+      <c r="A59" s="1">
+        <v>57</v>
+      </c>
+      <c r="B59" t="s">
+        <v>66</v>
+      </c>
+      <c r="C59">
+        <v>1676.610268005549</v>
+      </c>
+      <c r="D59">
+        <v>0.006999969482421875</v>
+      </c>
+      <c r="E59">
+        <v>7.11293361003758E-06</v>
+      </c>
+      <c r="F59">
+        <v>21.92482366701793</v>
+      </c>
+      <c r="G59">
+        <v>4.943173603449611</v>
+      </c>
+      <c r="H59">
+        <v>4.738617941974221</v>
+      </c>
+      <c r="I59">
+        <v>1347.510000000006</v>
+      </c>
+      <c r="J59">
+        <v>307.3800000000001</v>
+      </c>
+    </row>
+    <row r="60" spans="1:10">
+      <c r="A60" s="1">
+        <v>58</v>
+      </c>
+      <c r="B60" t="s">
+        <v>67</v>
+      </c>
+      <c r="C60">
+        <v>1014.423453125771</v>
+      </c>
+      <c r="D60">
+        <v>0.006000041961669922</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+      <c r="F60">
+        <v>22.00055025312762</v>
+      </c>
+      <c r="G60">
+        <v>5.894019291323108</v>
+      </c>
+      <c r="H60">
+        <v>3.646922163947599</v>
+      </c>
+      <c r="I60">
+        <v>793.1700000000191</v>
+      </c>
+      <c r="J60">
+        <v>201.5</v>
+      </c>
+    </row>
+    <row r="61" spans="1:10">
+      <c r="A61" s="1">
+        <v>59</v>
+      </c>
+      <c r="B61" t="s">
+        <v>68</v>
+      </c>
+      <c r="C61">
+        <v>391.2679608994313</v>
+      </c>
+      <c r="D61">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+      <c r="F61">
+        <v>23.91796089943222</v>
+      </c>
+      <c r="G61">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="H61">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="I61">
+        <v>218.7199999999991</v>
+      </c>
+      <c r="J61">
+        <v>148.63</v>
+      </c>
+    </row>
+    <row r="62" spans="1:10">
+      <c r="A62" s="1">
+        <v>60</v>
+      </c>
+      <c r="B62" t="s">
+        <v>69</v>
+      </c>
+      <c r="C62">
+        <v>77.8606459794474</v>
+      </c>
+      <c r="D62">
+        <v>0.0149998664855957</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+      <c r="F62">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G62">
+        <v>0</v>
+      </c>
+      <c r="H62">
+        <v>0</v>
+      </c>
+      <c r="I62">
+        <v>0</v>
+      </c>
+      <c r="J62">
+        <v>52.87</v>
+      </c>
+    </row>
+    <row r="63" spans="1:10">
+      <c r="A63" s="1">
+        <v>61</v>
+      </c>
+      <c r="B63" t="s">
+        <v>70</v>
+      </c>
+      <c r="C63">
+        <v>1674.399505879263</v>
+      </c>
+      <c r="D63">
+        <v>0.003999948501586914</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+      <c r="F63">
+        <v>23.33006819063954</v>
+      </c>
+      <c r="G63">
+        <v>6.41079396126198</v>
+      </c>
+      <c r="H63">
+        <v>2.590231649872266</v>
+      </c>
+      <c r="I63">
+        <v>1129.060000000013</v>
+      </c>
+      <c r="J63">
+        <v>525.83</v>
+      </c>
+    </row>
+    <row r="64" spans="1:10">
+      <c r="A64" s="1">
+        <v>62</v>
+      </c>
+      <c r="B64" t="s">
+        <v>71</v>
+      </c>
+      <c r="C64">
+        <v>147.3892770648809</v>
+      </c>
+      <c r="D64">
+        <v>0.004999876022338867</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+      <c r="F64">
+        <v>36.70927706488092</v>
+      </c>
+      <c r="G64">
+        <v>0</v>
+      </c>
+      <c r="H64">
+        <v>0</v>
+      </c>
+      <c r="I64">
+        <v>0</v>
+      </c>
+      <c r="J64">
+        <v>110.68</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
+      <c r="A65" s="1">
+        <v>63</v>
+      </c>
+      <c r="B65" t="s">
+        <v>72</v>
+      </c>
+      <c r="C65">
+        <v>307.6174397573979</v>
+      </c>
+      <c r="D65">
+        <v>181.175999879837</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+      <c r="F65">
+        <v>32.04743975738332</v>
+      </c>
+      <c r="G65">
+        <v>0</v>
+      </c>
+      <c r="H65">
+        <v>0</v>
+      </c>
+      <c r="I65">
+        <v>275.5700000000146</v>
+      </c>
+      <c r="J65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
+      <c r="A66" s="1">
+        <v>64</v>
+      </c>
+      <c r="B66" t="s">
+        <v>73</v>
+      </c>
+      <c r="C66">
+        <v>1017.797288545571</v>
+      </c>
+      <c r="D66">
+        <v>0.01200008392333984</v>
+      </c>
+      <c r="E66">
+        <v>0</v>
+      </c>
+      <c r="F66">
+        <v>26.35557902654179</v>
+      </c>
+      <c r="G66">
+        <v>8.443180413891367</v>
+      </c>
+      <c r="H66">
+        <v>5.214889932921746</v>
+      </c>
+      <c r="I66">
+        <v>691.7199999999982</v>
+      </c>
+      <c r="J66">
+        <v>302.95</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
+      <c r="A67" s="1">
+        <v>65</v>
+      </c>
+      <c r="B67" t="s">
+        <v>74</v>
+      </c>
+      <c r="C67">
+        <v>396.5896102867676</v>
+      </c>
+      <c r="D67">
+        <v>0.01099991798400879</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+      <c r="F67">
+        <v>27.5296102867676</v>
+      </c>
+      <c r="G67">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="H67">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="I67">
+        <v>275.55</v>
+      </c>
+      <c r="J67">
+        <v>93.50999999999999</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
+      <c r="A68" s="1">
+        <v>66</v>
+      </c>
+      <c r="B68" t="s">
+        <v>75</v>
+      </c>
+      <c r="C68">
+        <v>396.5896102867676</v>
+      </c>
+      <c r="D68">
+        <v>0.01200008392333984</v>
+      </c>
+      <c r="E68">
+        <v>0</v>
+      </c>
+      <c r="F68">
+        <v>27.5296102867676</v>
+      </c>
+      <c r="G68">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="H68">
+        <v>1.145862120850498</v>
+      </c>
+      <c r="I68">
+        <v>275.55</v>
+      </c>
+      <c r="J68">
+        <v>93.50999999999999</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
+      <c r="A69" s="1">
+        <v>67</v>
+      </c>
+      <c r="B69" t="s">
+        <v>76</v>
+      </c>
+      <c r="C69">
+        <v>357.4462074868381</v>
+      </c>
+      <c r="D69">
+        <v>0.01200008392333984</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+      <c r="F69">
+        <v>32.95620748683876</v>
+      </c>
+      <c r="G69">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="H69">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="I69">
+        <v>271.4099999999993</v>
+      </c>
+      <c r="J69">
+        <v>53.08</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
+      <c r="A70" s="1">
+        <v>68</v>
+      </c>
+      <c r="B70" t="s">
+        <v>77</v>
+      </c>
+      <c r="C70">
+        <v>1021.419132647999</v>
+      </c>
+      <c r="D70">
+        <v>0.009999990463256836</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+      <c r="F70">
+        <v>26.74913264799307</v>
+      </c>
+      <c r="G70">
+        <v>4.450188684067006</v>
+      </c>
+      <c r="H70">
+        <v>4.450188684067006</v>
+      </c>
+      <c r="I70">
+        <v>645.0300000000061</v>
+      </c>
+      <c r="J70">
+        <v>349.64</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
+      <c r="A71" s="1">
+        <v>69</v>
+      </c>
+      <c r="B71" t="s">
+        <v>78</v>
+      </c>
+      <c r="C71">
+        <v>651.7408010327504</v>
+      </c>
+      <c r="D71">
+        <v>0.01200008392333984</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+      <c r="F71">
+        <v>34.03080103274972</v>
+      </c>
+      <c r="G71">
+        <v>2.843170765184533</v>
+      </c>
+      <c r="H71">
+        <v>2.843170765184533</v>
+      </c>
+      <c r="I71">
+        <v>448.6400000000006</v>
+      </c>
+      <c r="J71">
+        <v>169.07</v>
+      </c>
+    </row>
+    <row r="72" spans="1:10">
+      <c r="A72" s="1">
+        <v>70</v>
+      </c>
+      <c r="B72" t="s">
+        <v>79</v>
+      </c>
+      <c r="C72">
+        <v>26.35557902654179</v>
+      </c>
+      <c r="D72">
+        <v>5.176999807357788</v>
+      </c>
+      <c r="E72">
+        <v>0</v>
+      </c>
+      <c r="F72">
+        <v>26.3555790265418</v>
+      </c>
+      <c r="G72">
+        <v>0</v>
+      </c>
+      <c r="H72">
+        <v>0</v>
+      </c>
+      <c r="I72">
+        <v>0</v>
+      </c>
+      <c r="J72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:10">
+      <c r="A73" s="1">
+        <v>71</v>
+      </c>
+      <c r="B73" t="s">
+        <v>80</v>
+      </c>
+      <c r="C73">
+        <v>1091.229339571329</v>
+      </c>
+      <c r="D73">
+        <v>0.00800013542175293</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+      <c r="F73">
+        <v>23.91796089943222</v>
+      </c>
+      <c r="G73">
+        <v>4.77723927008741</v>
+      </c>
+      <c r="H73">
+        <v>4.738617941974221</v>
+      </c>
+      <c r="I73">
+        <v>717.7100000000102</v>
+      </c>
+      <c r="J73">
+        <v>349.64</v>
+      </c>
+    </row>
+    <row r="74" spans="1:10">
+      <c r="A74" s="1">
+        <v>72</v>
+      </c>
+      <c r="B74" t="s">
+        <v>81</v>
+      </c>
+      <c r="C74">
+        <v>500.2806459794576</v>
+      </c>
+      <c r="D74">
+        <v>0.006999969482421875</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+      <c r="F74">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G74">
+        <v>2.378003364169193</v>
+      </c>
+      <c r="H74">
+        <v>2.378003364169193</v>
+      </c>
+      <c r="I74">
+        <v>235.9700000000101</v>
+      </c>
+      <c r="J74">
+        <v>239.32</v>
+      </c>
+    </row>
+    <row r="75" spans="1:10">
+      <c r="A75" s="1">
+        <v>73</v>
+      </c>
+      <c r="B75" t="s">
+        <v>82</v>
+      </c>
+      <c r="C75">
+        <v>500.2806459794576</v>
+      </c>
+      <c r="D75">
+        <v>0.008999824523925781</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+      <c r="F75">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G75">
+        <v>2.378003364169193</v>
+      </c>
+      <c r="H75">
+        <v>2.378003364169193</v>
+      </c>
+      <c r="I75">
+        <v>235.9700000000101</v>
+      </c>
+      <c r="J75">
+        <v>239.32</v>
+      </c>
+    </row>
+    <row r="76" spans="1:10">
+      <c r="A76" s="1">
+        <v>74</v>
+      </c>
+      <c r="B76" t="s">
+        <v>83</v>
+      </c>
+      <c r="C76">
+        <v>26.35557902654179</v>
+      </c>
+      <c r="D76">
+        <v>0.004999876022338867</v>
+      </c>
+      <c r="E76">
+        <v>0</v>
+      </c>
+      <c r="F76">
+        <v>26.35557902654179</v>
+      </c>
+      <c r="G76">
+        <v>0</v>
+      </c>
+      <c r="H76">
+        <v>0</v>
+      </c>
+      <c r="I76">
+        <v>0</v>
+      </c>
+      <c r="J76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:10">
+      <c r="A77" s="1">
+        <v>75</v>
+      </c>
+      <c r="B77" t="s">
+        <v>84</v>
+      </c>
+      <c r="C77">
+        <v>1091.321310081332</v>
+      </c>
+      <c r="D77">
+        <v>0.009000062942504883</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+      <c r="F77">
+        <v>24.3115145208835</v>
+      </c>
+      <c r="G77">
+        <v>3.754788217841379</v>
+      </c>
+      <c r="H77">
+        <v>3.414583778284226</v>
+      </c>
+      <c r="I77">
+        <v>1014.270000000005</v>
+      </c>
+      <c r="J77">
+        <v>53.08</v>
+      </c>
+    </row>
+    <row r="78" spans="1:10">
+      <c r="A78" s="1">
+        <v>76</v>
+      </c>
+      <c r="B78" t="s">
+        <v>85</v>
+      </c>
+      <c r="C78">
+        <v>142.7308010327497</v>
+      </c>
+      <c r="D78">
+        <v>0.004999876022338867</v>
+      </c>
+      <c r="E78">
+        <v>0</v>
+      </c>
+      <c r="F78">
+        <v>34.03080103274972</v>
+      </c>
+      <c r="G78">
+        <v>0</v>
+      </c>
+      <c r="H78">
+        <v>0</v>
+      </c>
+      <c r="I78">
+        <v>0</v>
+      </c>
+      <c r="J78">
+        <v>108.7</v>
+      </c>
+    </row>
+    <row r="79" spans="1:10">
+      <c r="A79" s="1">
+        <v>77</v>
+      </c>
+      <c r="B79" t="s">
+        <v>86</v>
+      </c>
+      <c r="C79">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="D79">
+        <v>5.861999988555908</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+      <c r="F79">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G79">
+        <v>0</v>
+      </c>
+      <c r="H79">
+        <v>0</v>
+      </c>
+      <c r="I79">
+        <v>0</v>
+      </c>
+      <c r="J79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:10">
+      <c r="A80" s="1">
+        <v>78</v>
+      </c>
+      <c r="B80" t="s">
+        <v>87</v>
+      </c>
+      <c r="C80">
+        <v>1676.610268005544</v>
+      </c>
+      <c r="D80">
+        <v>0.007999897003173828</v>
+      </c>
+      <c r="E80">
+        <v>6.830343646905243E-06</v>
+      </c>
+      <c r="F80">
+        <v>21.92482366701793</v>
+      </c>
+      <c r="G80">
+        <v>4.943173603449611</v>
+      </c>
+      <c r="H80">
+        <v>4.738617941974221</v>
+      </c>
+      <c r="I80">
+        <v>1436.870000000001</v>
+      </c>
+      <c r="J80">
+        <v>218.02</v>
+      </c>
+    </row>
+    <row r="81" spans="1:10">
+      <c r="A81" s="1">
+        <v>79</v>
+      </c>
+      <c r="B81" t="s">
+        <v>88</v>
+      </c>
+      <c r="C81">
+        <v>1013.861678843903</v>
+      </c>
+      <c r="D81">
+        <v>0.007999897003173828</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+      <c r="F81">
+        <v>22.00055025312762</v>
+      </c>
+      <c r="G81">
+        <v>6.773023273111587</v>
+      </c>
+      <c r="H81">
+        <v>3.9641518638922</v>
+      </c>
+      <c r="I81">
+        <v>846.039999999995</v>
+      </c>
+      <c r="J81">
+        <v>148.63</v>
+      </c>
+    </row>
+    <row r="82" spans="1:10">
+      <c r="A82" s="1">
+        <v>80</v>
+      </c>
+      <c r="B82" t="s">
+        <v>89</v>
+      </c>
+      <c r="C82">
+        <v>391.2525123681869</v>
+      </c>
+      <c r="D82">
+        <v>0.009000062942504883</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+      <c r="F82">
+        <v>23.91796089943222</v>
+      </c>
+      <c r="G82">
+        <v>2.598412980545262</v>
+      </c>
+      <c r="H82">
+        <v>2.582964449299987</v>
+      </c>
+      <c r="I82">
+        <v>367.35</v>
+      </c>
+      <c r="J82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:10">
+      <c r="A83" s="1">
+        <v>81</v>
+      </c>
+      <c r="B83" t="s">
+        <v>90</v>
+      </c>
+      <c r="C83">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="D83">
+        <v>0.006000041961669922</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+      <c r="F83">
+        <v>24.99064597944741</v>
+      </c>
+      <c r="G83">
+        <v>0</v>
+      </c>
+      <c r="H83">
+        <v>0</v>
+      </c>
+      <c r="I83">
+        <v>0</v>
+      </c>
+      <c r="J83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:10">
+      <c r="A84" s="1">
+        <v>82</v>
+      </c>
+      <c r="B84" t="s">
+        <v>91</v>
+      </c>
+      <c r="C84">
+        <v>1674.399505879249</v>
+      </c>
+      <c r="D84">
+        <v>0.007999897003173828</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+      <c r="F84">
+        <v>23.33006819063954</v>
+      </c>
+      <c r="G84">
+        <v>6.41079396126198</v>
+      </c>
+      <c r="H84">
+        <v>2.590231649872266</v>
+      </c>
+      <c r="I84">
+        <v>1384.939999999999</v>
+      </c>
+      <c r="J84">
+        <v>269.95</v>
+      </c>
+    </row>
+    <row r="85" spans="1:10">
+      <c r="A85" s="1">
+        <v>83</v>
+      </c>
+      <c r="B85" t="s">
+        <v>92</v>
+      </c>
+      <c r="C85">
+        <v>142.7308010327497</v>
+      </c>
+      <c r="D85">
+        <v>0.006000041961669922</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+      <c r="F85">
+        <v>34.03080103274972</v>
+      </c>
+      <c r="G85">
+        <v>0</v>
+      </c>
+      <c r="H85">
+        <v>0</v>
+      </c>
+      <c r="I85">
+        <v>0</v>
+      </c>
+      <c r="J85">
+        <v>108.7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>